<commit_message>
update visualization of grocery related data
</commit_message>
<xml_diff>
--- a/Grocery_Data.xlsx
+++ b/Grocery_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/erl88_pitt_edu/Documents/Notability/A Fall 2025/CS 0010/Final_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/erl88_pitt_edu/Documents/Notability/A Fall 2025/CS 0010/Final_Project-CMPINF0010/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_F25DC773A252ABDACC1048F9899C53345ADE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC987A1D-FD09-4C54-A89A-4559B2C730B9}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="11_F25DC773A252ABDACC1048F9899C53345ADE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E04E3F5-9B1D-4BF6-B1E7-160800465062}"/>
   <bookViews>
-    <workbookView xWindow="12067" yWindow="0" windowWidth="12315" windowHeight="15563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="24">
   <si>
     <t>Zip</t>
   </si>
@@ -71,9 +71,6 @@
     <t>West Mifflin</t>
   </si>
   <si>
-    <t>Troy Hill</t>
-  </si>
-  <si>
     <t>East Liberty</t>
   </si>
   <si>
@@ -93,6 +90,24 @@
   </si>
   <si>
     <t>Strip District</t>
+  </si>
+  <si>
+    <t>Lawrenceville</t>
+  </si>
+  <si>
+    <t>Mt. Lebanon</t>
+  </si>
+  <si>
+    <t>O'Hara Township</t>
+  </si>
+  <si>
+    <t>Heidelberg</t>
+  </si>
+  <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
@@ -140,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,6 +167,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -173,6 +210,2002 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$U$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$T$8:$T$17</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Strip District</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>East Liberty</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Squirrel Hill </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ross Township</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Heidelberg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>South Side Slopes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mt. Lebanon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>O'Hara Township</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lawrenceville</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Shadyside </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$8:$U$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5D91-435B-810D-42126D34ECBB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="654760032"/>
+        <c:axId val="654758592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="654760032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654758592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="654758592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654760032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Grocery</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> &amp; Convenient Store Number</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grocery</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$X$8:$X$17</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Strip District</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>East Liberty</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Squirrel Hill </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ross Township</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Heidelberg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>South Side Slopes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mt. Lebanon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>O'Hara Township</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lawrenceville</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Shadyside </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$8:$Y$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5C6E-42E2-9BA0-12A9E04887CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Convenient Store</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$X$8:$X$17</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Strip District</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>East Liberty</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Squirrel Hill </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Ross Township</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Heidelberg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>South Side Slopes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mt. Lebanon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>O'Hara Township</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lawrenceville</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Shadyside </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$8:$Z$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5C6E-42E2-9BA0-12A9E04887CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="760242608"/>
+        <c:axId val="760243688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="760242608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="760243688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="760243688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="760242608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>373062</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108744</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>55562</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>113506</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F037DCF-D2B6-12ED-3C97-7394263EDC79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>162719</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>116681</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>456407</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>121443</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A9C5833-7BB3-0B31-65D3-34ABC4E67E54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
+<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
+  <bag type="Checkbox"/>
+  <bag type="XFControls">
+    <bagId k="CellControl">0</bagId>
+  </bag>
+  <bag type="XFComplement">
+    <bagId k="XFControls">1</bagId>
+  </bag>
+  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
+    <a k="MappedFeaturePropertyBags">
+      <bagId>2</bagId>
+    </a>
+  </bag>
+</FeaturePropertyBags>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,15 +2471,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +2505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>15237</v>
       </c>
@@ -502,7 +2535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>15146</v>
       </c>
@@ -532,7 +2565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>15132</v>
       </c>
@@ -562,7 +2595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>15122</v>
       </c>
@@ -592,37 +2625,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6">
+    <row r="6" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>15222</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>21</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>15222</v>
       </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
         <v>15222</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>17</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>15205</v>
       </c>
@@ -648,8 +2681,32 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="O7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" t="s">
+        <v>23</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>15210</v>
       </c>
@@ -675,8 +2732,48 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="L8" s="2">
+        <v>15222</v>
+      </c>
+      <c r="M8" s="2">
+        <v>21</v>
+      </c>
+      <c r="N8" s="2">
+        <v>15222</v>
+      </c>
+      <c r="O8" s="8">
+        <v>4</v>
+      </c>
+      <c r="P8" s="2">
+        <v>15222</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>17</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" ref="S8" si="1" xml:space="preserve"> 3*O8+1*Q8</f>
+        <v>29</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="U8">
+        <v>29</v>
+      </c>
+      <c r="X8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>4</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>15235</v>
       </c>
@@ -702,8 +2799,48 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="L9" s="2">
+        <v>15206</v>
+      </c>
+      <c r="M9" s="2">
+        <v>17</v>
+      </c>
+      <c r="N9" s="2">
+        <v>15206</v>
+      </c>
+      <c r="O9" s="8">
+        <v>4</v>
+      </c>
+      <c r="P9" s="2">
+        <v>15206</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>13</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S9" s="2">
+        <f xml:space="preserve"> 3*O9+1*Q9</f>
+        <v>25</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="U9">
+        <v>25</v>
+      </c>
+      <c r="X9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y9" s="8">
+        <v>4</v>
+      </c>
+      <c r="Z9" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>15108</v>
       </c>
@@ -729,8 +2866,48 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="L10" s="4">
+        <v>15217</v>
+      </c>
+      <c r="M10" s="4">
+        <v>11</v>
+      </c>
+      <c r="N10" s="4">
+        <v>15217</v>
+      </c>
+      <c r="O10" s="9">
+        <v>4</v>
+      </c>
+      <c r="P10" s="4">
+        <v>15217</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>7</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" ref="S10:S17" si="2" xml:space="preserve"> 3*O10+1*Q10</f>
+        <v>19</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10">
+        <v>19</v>
+      </c>
+      <c r="X10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y10" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>15206</v>
       </c>
@@ -753,14 +2930,54 @@
         <v>4</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> 3*D11+1*F11</f>
         <v>25</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+      <c r="L11" s="2">
+        <v>15224</v>
+      </c>
+      <c r="M11" s="2">
+        <v>11</v>
+      </c>
+      <c r="N11" s="2">
+        <v>15224</v>
+      </c>
+      <c r="O11" s="8">
+        <v>3</v>
+      </c>
+      <c r="P11" s="2">
+        <v>15224</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>8</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="U11" s="2">
+        <v>17</v>
+      </c>
+      <c r="X11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y11" s="8">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>15227</v>
       </c>
@@ -786,8 +3003,48 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="L12" s="4">
+        <v>15106</v>
+      </c>
+      <c r="M12" s="4">
+        <v>9</v>
+      </c>
+      <c r="N12" s="4">
+        <v>15106</v>
+      </c>
+      <c r="O12" s="9">
+        <v>3</v>
+      </c>
+      <c r="P12" s="4">
+        <v>15106</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>6</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="U12">
+        <v>15</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y12" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z12" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>15236</v>
       </c>
@@ -813,8 +3070,48 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="L13" s="2">
+        <v>15203</v>
+      </c>
+      <c r="M13" s="2">
+        <v>8</v>
+      </c>
+      <c r="N13" s="2">
+        <v>15203</v>
+      </c>
+      <c r="O13" s="8">
+        <v>2</v>
+      </c>
+      <c r="P13" s="2">
+        <v>15203</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>6</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="U13">
+        <v>12</v>
+      </c>
+      <c r="X13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>15212</v>
       </c>
@@ -840,8 +3137,48 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="L14" s="2">
+        <v>15216</v>
+      </c>
+      <c r="M14" s="2">
+        <v>7</v>
+      </c>
+      <c r="N14" s="2">
+        <v>15216</v>
+      </c>
+      <c r="O14" s="8">
+        <v>2</v>
+      </c>
+      <c r="P14" s="2">
+        <v>15216</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>5</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="T14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="U14" s="6">
+        <v>11</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>15213</v>
       </c>
@@ -867,8 +3204,48 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="L15" s="2">
+        <v>15116</v>
+      </c>
+      <c r="M15" s="2">
+        <v>6</v>
+      </c>
+      <c r="N15" s="2">
+        <v>15116</v>
+      </c>
+      <c r="O15" s="8">
+        <v>2</v>
+      </c>
+      <c r="P15" s="2">
+        <v>15116</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>4</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="U15">
+        <v>10</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y15" s="8">
+        <v>2</v>
+      </c>
+      <c r="Z15" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15221</v>
       </c>
@@ -895,10 +3272,50 @@
         <v>22</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="L16" s="2">
+        <v>15201</v>
+      </c>
+      <c r="M16" s="2">
+        <v>7</v>
+      </c>
+      <c r="N16" s="2">
+        <v>15201</v>
+      </c>
+      <c r="O16" s="8">
+        <v>1</v>
+      </c>
+      <c r="P16" s="2">
+        <v>15201</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>6</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="U16">
+        <v>9</v>
+      </c>
+      <c r="X16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y16" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15090</v>
       </c>
@@ -924,8 +3341,48 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="L17" s="4">
+        <v>15232</v>
+      </c>
+      <c r="M17" s="4">
+        <v>4</v>
+      </c>
+      <c r="N17" s="4">
+        <v>15232</v>
+      </c>
+      <c r="O17" s="9">
+        <v>1</v>
+      </c>
+      <c r="P17" s="4">
+        <v>15232</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>3</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="U17">
+        <v>6</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y17" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>15136</v>
       </c>
@@ -952,7 +3409,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>15147</v>
       </c>
@@ -979,7 +3436,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>15217</v>
       </c>
@@ -1006,10 +3463,10 @@
         <v>19</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>15219</v>
       </c>
@@ -1036,7 +3493,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>15044</v>
       </c>
@@ -1063,7 +3520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>15224</v>
       </c>
@@ -1090,10 +3547,10 @@
         <v>17</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>15102</v>
       </c>
@@ -1120,7 +3577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>15120</v>
       </c>
@@ -1147,7 +3604,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>15017</v>
       </c>
@@ -1174,34 +3631,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27">
+    <row r="27" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
         <v>15106</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="4">
         <v>9</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <v>15106</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>3</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>15106</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="4">
         <v>6</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27">
+      <c r="G27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I27" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>15137</v>
       </c>
@@ -1228,7 +3688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>15238</v>
       </c>
@@ -1255,7 +3715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>15229</v>
       </c>
@@ -1282,7 +3742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>15084</v>
       </c>
@@ -1309,7 +3769,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15101</v>
       </c>
@@ -1336,7 +3796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>15203</v>
       </c>
@@ -1363,10 +3823,10 @@
         <v>12</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>15220</v>
       </c>
@@ -1389,11 +3849,11 @@
         <v>4</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H65" si="1" xml:space="preserve"> 3*D34+1*F34</f>
+        <f t="shared" ref="H34:H65" si="3" xml:space="preserve"> 3*D34+1*F34</f>
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>15226</v>
       </c>
@@ -1416,11 +3876,11 @@
         <v>4</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>15202</v>
       </c>
@@ -1443,38 +3903,41 @@
         <v>4</v>
       </c>
       <c r="H36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A37">
+    <row r="37" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
         <v>15216</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>7</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>15216</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>2</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>15216</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>5</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="1"/>
+      <c r="G37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I37" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>15037</v>
       </c>
@@ -1497,11 +3960,11 @@
         <v>4</v>
       </c>
       <c r="H38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>15071</v>
       </c>
@@ -1524,38 +3987,41 @@
         <v>4</v>
       </c>
       <c r="H39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A40">
+    <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
         <v>15116</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>6</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>15116</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>2</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>15116</v>
       </c>
-      <c r="F40">
-        <v>4</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="1"/>
+      <c r="F40" s="2">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I40" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>15131</v>
       </c>
@@ -1578,11 +4044,11 @@
         <v>4</v>
       </c>
       <c r="H41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>15218</v>
       </c>
@@ -1605,11 +4071,11 @@
         <v>4</v>
       </c>
       <c r="H42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>15228</v>
       </c>
@@ -1632,11 +4098,11 @@
         <v>4</v>
       </c>
       <c r="H43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>15241</v>
       </c>
@@ -1659,11 +4125,11 @@
         <v>4</v>
       </c>
       <c r="H44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>15065</v>
       </c>
@@ -1686,11 +4152,11 @@
         <v>4</v>
       </c>
       <c r="H45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>15201</v>
       </c>
@@ -1713,14 +4179,14 @@
         <v>4</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>15208</v>
       </c>
@@ -1743,11 +4209,11 @@
         <v>4</v>
       </c>
       <c r="H47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>15234</v>
       </c>
@@ -1770,11 +4236,11 @@
         <v>4</v>
       </c>
       <c r="H48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>15239</v>
       </c>
@@ -1797,11 +4263,11 @@
         <v>4</v>
       </c>
       <c r="H49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>15143</v>
       </c>
@@ -1824,11 +4290,11 @@
         <v>4</v>
       </c>
       <c r="H50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>15211</v>
       </c>
@@ -1851,11 +4317,11 @@
         <v>4</v>
       </c>
       <c r="H51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>15104</v>
       </c>
@@ -1878,11 +4344,11 @@
         <v>4</v>
       </c>
       <c r="H52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>15110</v>
       </c>
@@ -1905,11 +4371,11 @@
         <v>4</v>
       </c>
       <c r="H53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>15145</v>
       </c>
@@ -1932,11 +4398,11 @@
         <v>4</v>
       </c>
       <c r="H54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>15209</v>
       </c>
@@ -1959,11 +4425,11 @@
         <v>4</v>
       </c>
       <c r="H55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>15215</v>
       </c>
@@ -1986,11 +4452,11 @@
         <v>4</v>
       </c>
       <c r="H56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>15232</v>
       </c>
@@ -2013,14 +4479,14 @@
         <v>4</v>
       </c>
       <c r="H57" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>15275</v>
       </c>
@@ -2043,11 +4509,11 @@
         <v>4</v>
       </c>
       <c r="H58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>15025</v>
       </c>
@@ -2070,11 +4536,11 @@
         <v>4</v>
       </c>
       <c r="H59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>15139</v>
       </c>
@@ -2097,11 +4563,11 @@
         <v>4</v>
       </c>
       <c r="H60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>15223</v>
       </c>
@@ -2124,11 +4590,11 @@
         <v>4</v>
       </c>
       <c r="H61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>15024</v>
       </c>
@@ -2151,11 +4617,11 @@
         <v>4</v>
       </c>
       <c r="H62">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>15056</v>
       </c>
@@ -2178,11 +4644,11 @@
         <v>4</v>
       </c>
       <c r="H63">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>15086</v>
       </c>
@@ -2205,11 +4671,11 @@
         <v>4</v>
       </c>
       <c r="H64">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>15207</v>
       </c>
@@ -2232,11 +4698,11 @@
         <v>4</v>
       </c>
       <c r="H65">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>15076</v>
       </c>
@@ -2259,11 +4725,11 @@
         <v>4</v>
       </c>
       <c r="H66">
-        <f t="shared" ref="H66:H91" si="2" xml:space="preserve"> 3*D66+1*F66</f>
+        <f t="shared" ref="H66:H91" si="4" xml:space="preserve"> 3*D66+1*F66</f>
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>15112</v>
       </c>
@@ -2286,11 +4752,11 @@
         <v>4</v>
       </c>
       <c r="H67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>15127</v>
       </c>
@@ -2313,11 +4779,11 @@
         <v>4</v>
       </c>
       <c r="H68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>15204</v>
       </c>
@@ -2340,11 +4806,11 @@
         <v>4</v>
       </c>
       <c r="H69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>15214</v>
       </c>
@@ -2367,11 +4833,11 @@
         <v>4</v>
       </c>
       <c r="H70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>15233</v>
       </c>
@@ -2394,11 +4860,11 @@
         <v>4</v>
       </c>
       <c r="H71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>15014</v>
       </c>
@@ -2421,11 +4887,11 @@
         <v>4</v>
       </c>
       <c r="H72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>15026</v>
       </c>
@@ -2448,11 +4914,11 @@
         <v>4</v>
       </c>
       <c r="H73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>15045</v>
       </c>
@@ -2475,11 +4941,11 @@
         <v>4</v>
       </c>
       <c r="H74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>15088</v>
       </c>
@@ -2502,11 +4968,11 @@
         <v>4</v>
       </c>
       <c r="H75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>15129</v>
       </c>
@@ -2529,11 +4995,11 @@
         <v>4</v>
       </c>
       <c r="H76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>15140</v>
       </c>
@@ -2556,11 +5022,11 @@
         <v>4</v>
       </c>
       <c r="H77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>15225</v>
       </c>
@@ -2583,11 +5049,11 @@
         <v>4</v>
       </c>
       <c r="H78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>15018</v>
       </c>
@@ -2610,11 +5076,11 @@
         <v>4</v>
       </c>
       <c r="H79">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>15030</v>
       </c>
@@ -2637,11 +5103,11 @@
         <v>4</v>
       </c>
       <c r="H80">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>15034</v>
       </c>
@@ -2664,11 +5130,11 @@
         <v>4</v>
       </c>
       <c r="H81">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>15035</v>
       </c>
@@ -2691,11 +5157,11 @@
         <v>4</v>
       </c>
       <c r="H82">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>15046</v>
       </c>
@@ -2718,11 +5184,11 @@
         <v>4</v>
       </c>
       <c r="H83">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>15057</v>
       </c>
@@ -2745,11 +5211,11 @@
         <v>4</v>
       </c>
       <c r="H84">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>15133</v>
       </c>
@@ -2772,11 +5238,11 @@
         <v>4</v>
       </c>
       <c r="H85">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>15135</v>
       </c>
@@ -2799,11 +5265,11 @@
         <v>4</v>
       </c>
       <c r="H86">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>15142</v>
       </c>
@@ -2826,11 +5292,11 @@
         <v>4</v>
       </c>
       <c r="H87">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>15144</v>
       </c>
@@ -2853,11 +5319,11 @@
         <v>4</v>
       </c>
       <c r="H88">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>15231</v>
       </c>
@@ -2880,11 +5346,11 @@
         <v>4</v>
       </c>
       <c r="H89">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>15282</v>
       </c>
@@ -2907,11 +5373,11 @@
         <v>4</v>
       </c>
       <c r="H90">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>16046</v>
       </c>
@@ -2934,7 +5400,7 @@
         <v>4</v>
       </c>
       <c r="H91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2943,5 +5409,6 @@
     <sortCondition descending="1" ref="H2:H91"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>